<commit_message>
Added Neural Network Code
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -130,7 +131,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,13 +139,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -159,8 +187,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -466,7 +499,7 @@
     <col min="1" max="1" width="12.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
@@ -475,570 +508,1668 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2">
+      <c r="A2" s="5">
         <v>2014</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>35</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>300</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>22</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>57</v>
       </c>
-      <c r="H2">
-        <v>258391402.273</v>
+      <c r="H2" s="2">
+        <v>258.39140229999998</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="B3" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>80</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>300</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>25</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>51</v>
       </c>
-      <c r="H3">
-        <v>9100000000</v>
+      <c r="H3" s="2">
+        <v>9100</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="C4" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>70</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>200</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>27</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>53</v>
       </c>
-      <c r="H4">
-        <v>4949000000</v>
+      <c r="H4" s="2">
+        <v>4949</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="B5" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>45</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>250</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>22</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>62</v>
       </c>
-      <c r="H5">
-        <f>12280452.05+10010.1+29000</f>
-        <v>12319462.15</v>
+      <c r="H5" s="2">
+        <v>12.31946215</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="C6" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>45</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>250</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>23</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>60</v>
       </c>
-      <c r="H6">
-        <v>606529</v>
+      <c r="H6" s="2">
+        <v>0.60652899999999998</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="B7" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>65</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>200</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>22</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>62</v>
       </c>
-      <c r="H7">
-        <v>365638470</v>
+      <c r="H7" s="2">
+        <v>365.63846999999998</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="B8" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>90</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>250</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>19</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>59</v>
       </c>
-      <c r="H8">
-        <v>301162911</v>
+      <c r="H8" s="2">
+        <v>301.16291100000001</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="C9" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>90</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>250</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>18</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>61</v>
       </c>
-      <c r="H9">
-        <v>262083045</v>
+      <c r="H9" s="2">
+        <v>262.08304500000003</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="C10" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>45</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>112</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>27</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>53</v>
       </c>
-      <c r="H10">
-        <v>17611663</v>
+      <c r="H10" s="2">
+        <v>17.611663</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="B11" t="s">
+      <c r="A11" s="5"/>
+      <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>35</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>175</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>18</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>57</v>
       </c>
-      <c r="H11">
-        <v>31905967.289999999</v>
+      <c r="H11" s="2">
+        <v>31.90596729</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="C12" t="s">
+      <c r="A12" s="5"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>40</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>200</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>20</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>58</v>
       </c>
-      <c r="H12">
-        <v>52504807</v>
+      <c r="H12" s="2">
+        <v>52.504807</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="C13" t="s">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>35</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>200</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>21</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>61</v>
       </c>
-      <c r="H13">
-        <v>489040</v>
+      <c r="H13" s="2">
+        <v>0.48903999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14">
+      <c r="A14" s="5">
         <v>2013</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>35</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>250</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>19</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>59</v>
       </c>
-      <c r="H14">
-        <v>31220989</v>
+      <c r="H14" s="2">
+        <v>31.220988999999999</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="C15" t="s">
+      <c r="A15" s="5"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>35</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>300</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>18</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="2">
         <v>57</v>
       </c>
-      <c r="H15">
-        <v>44782100</v>
+      <c r="H15" s="2">
+        <v>44.7821</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="C16" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>35</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>250</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>27</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>53</v>
       </c>
-      <c r="H16">
-        <v>11745100</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" t="s">
+      <c r="H16" s="2">
+        <v>11.745100000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="5"/>
+      <c r="B17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>35</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>200</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>22</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2">
         <v>62</v>
       </c>
-      <c r="H17">
-        <v>36282100</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" t="s">
+      <c r="H17" s="2">
+        <v>36.2821</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="5"/>
+      <c r="B18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>95</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>350</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>17</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>58</v>
       </c>
-      <c r="H18">
-        <f>398073951+32828259</f>
-        <v>430902210</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="C19" t="s">
+      <c r="H18" s="2">
+        <v>430.90221000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="5"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>75</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>350</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>24</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <v>53</v>
       </c>
-      <c r="H19">
-        <f>2200000+11912070</f>
-        <v>14112070</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8">
-      <c r="B20" t="s">
+      <c r="H19" s="2">
+        <v>14.112069999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="5"/>
+      <c r="B20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>70</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>400</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>17</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="2">
         <v>58</v>
       </c>
-      <c r="H20">
-        <v>59283222</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="C21" t="s">
+      <c r="H20" s="2">
+        <v>59.283222000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>65</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>320</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>19</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="2">
         <v>66</v>
       </c>
-      <c r="H21">
-        <v>3845216</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8">
-      <c r="B22" t="s">
+      <c r="H21" s="2">
+        <v>3.8452160000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="5"/>
+      <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>70</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>52</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>22</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="2">
         <v>62</v>
       </c>
-      <c r="H22">
-        <f>180877580+2061500</f>
-        <v>182939080</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8">
-      <c r="C23" t="s">
+      <c r="H22" s="2">
+        <v>182.93907999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="5"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="2">
         <v>70</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <v>52</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <v>23</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="2">
         <v>60</v>
       </c>
-      <c r="H23">
-        <v>235031910.46000001</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8">
-      <c r="B24" t="s">
+      <c r="H23" s="2">
+        <v>235.03191050000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="5"/>
+      <c r="B24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="2">
         <v>110</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>52</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>20</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="2">
         <v>57</v>
       </c>
-      <c r="H24">
-        <v>2665705225</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8">
-      <c r="C25" t="s">
+      <c r="H24" s="2">
+        <v>2665.7052250000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="5"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
         <v>90</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>52</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>22</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="2">
         <v>64</v>
       </c>
-      <c r="H25">
-        <v>537856800</v>
-      </c>
+      <c r="H25" s="2">
+        <v>537.85680000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="5"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="B31" s="2"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="2:8">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="2"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+    </row>
+    <row r="38" spans="2:8">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="2"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:BC40"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3:AE32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="18:55">
+      <c r="R1" s="3"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="3"/>
+      <c r="AL1" s="3"/>
+      <c r="AM1" s="3"/>
+      <c r="AN1" s="3"/>
+      <c r="AO1" s="3"/>
+      <c r="AP1" s="3"/>
+      <c r="AQ1" s="3"/>
+      <c r="AR1" s="3"/>
+      <c r="AS1" s="3"/>
+      <c r="AT1" s="3"/>
+      <c r="AU1" s="3"/>
+      <c r="AV1" s="3"/>
+      <c r="AW1" s="3"/>
+      <c r="AX1" s="3"/>
+      <c r="AY1" s="3"/>
+      <c r="AZ1" s="3"/>
+      <c r="BA1" s="3"/>
+      <c r="BB1" s="3"/>
+      <c r="BC1" s="3"/>
+    </row>
+    <row r="2" spans="18:55">
+      <c r="R2" s="3"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
+      <c r="AK2" s="3"/>
+      <c r="AL2" s="3"/>
+      <c r="AM2" s="3"/>
+      <c r="AN2" s="3"/>
+      <c r="AO2" s="3"/>
+      <c r="AP2" s="3"/>
+      <c r="AQ2" s="3"/>
+      <c r="AR2" s="3"/>
+      <c r="AS2" s="3"/>
+      <c r="AT2" s="3"/>
+      <c r="AU2" s="3"/>
+      <c r="AV2" s="3"/>
+      <c r="AW2" s="3"/>
+      <c r="AX2" s="3"/>
+      <c r="AY2" s="3"/>
+      <c r="AZ2" s="3"/>
+      <c r="BA2" s="3"/>
+      <c r="BB2" s="3"/>
+      <c r="BC2" s="3"/>
+    </row>
+    <row r="3" spans="18:55">
+      <c r="R3" s="3"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="2"/>
+      <c r="AU3" s="2"/>
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="2"/>
+    </row>
+    <row r="4" spans="18:55">
+      <c r="R4" s="3"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2"/>
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="2"/>
+      <c r="AS4" s="2"/>
+      <c r="AT4" s="2"/>
+      <c r="AU4" s="2"/>
+      <c r="AV4" s="2"/>
+      <c r="AW4" s="2"/>
+      <c r="AX4" s="2"/>
+      <c r="AY4" s="2"/>
+      <c r="AZ4" s="2"/>
+      <c r="BA4" s="2"/>
+      <c r="BB4" s="2"/>
+      <c r="BC4" s="2"/>
+    </row>
+    <row r="5" spans="18:55">
+      <c r="R5" s="3"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="3"/>
+      <c r="AK5" s="3"/>
+      <c r="AL5" s="3"/>
+      <c r="AM5" s="3"/>
+      <c r="AN5" s="3"/>
+      <c r="AO5" s="3"/>
+      <c r="AP5" s="3"/>
+      <c r="AQ5" s="3"/>
+      <c r="AR5" s="3"/>
+      <c r="AS5" s="3"/>
+      <c r="AT5" s="3"/>
+      <c r="AU5" s="3"/>
+      <c r="AV5" s="3"/>
+      <c r="AW5" s="3"/>
+      <c r="AX5" s="3"/>
+      <c r="AY5" s="3"/>
+      <c r="AZ5" s="3"/>
+      <c r="BA5" s="3"/>
+      <c r="BB5" s="3"/>
+      <c r="BC5" s="3"/>
+    </row>
+    <row r="6" spans="18:55">
+      <c r="R6" s="3"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="4"/>
+      <c r="AP6" s="4"/>
+      <c r="AQ6" s="4"/>
+      <c r="AR6" s="4"/>
+      <c r="AS6" s="4"/>
+    </row>
+    <row r="7" spans="18:55">
+      <c r="R7" s="3"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="3"/>
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="4"/>
+      <c r="AP7" s="4"/>
+      <c r="AQ7" s="4"/>
+      <c r="AR7" s="4"/>
+      <c r="AS7" s="4"/>
+    </row>
+    <row r="8" spans="18:55">
+      <c r="R8" s="3"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="3"/>
+      <c r="AK8" s="3"/>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="3"/>
+      <c r="AN8" s="2"/>
+      <c r="AO8" s="4"/>
+      <c r="AP8" s="4"/>
+      <c r="AQ8" s="4"/>
+      <c r="AR8" s="4"/>
+      <c r="AS8" s="4"/>
+    </row>
+    <row r="9" spans="18:55">
+      <c r="R9" s="3"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="AI9" s="3"/>
+      <c r="AJ9" s="3"/>
+      <c r="AK9" s="3"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="3"/>
+      <c r="AN9" s="2"/>
+    </row>
+    <row r="10" spans="18:55">
+      <c r="R10" s="3"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="3"/>
+      <c r="AL10" s="2"/>
+      <c r="AM10" s="3"/>
+      <c r="AN10" s="2"/>
+    </row>
+    <row r="11" spans="18:55">
+      <c r="R11" s="3"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="AI11" s="3"/>
+      <c r="AJ11" s="3"/>
+      <c r="AK11" s="3"/>
+      <c r="AL11" s="2"/>
+      <c r="AM11" s="3"/>
+      <c r="AN11" s="2"/>
+    </row>
+    <row r="12" spans="18:55">
+      <c r="R12" s="3"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Y12" s="3"/>
+      <c r="AI12" s="3"/>
+      <c r="AJ12" s="3"/>
+      <c r="AK12" s="3"/>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="3"/>
+      <c r="AN12" s="2"/>
+    </row>
+    <row r="13" spans="18:55">
+      <c r="R13" s="3"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3"/>
+      <c r="AI13" s="3"/>
+      <c r="AJ13" s="3"/>
+      <c r="AK13" s="3"/>
+      <c r="AL13" s="2"/>
+      <c r="AM13" s="3"/>
+      <c r="AN13" s="2"/>
+    </row>
+    <row r="14" spans="18:55">
+      <c r="R14" s="3"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="AI14" s="3"/>
+      <c r="AJ14" s="3"/>
+      <c r="AK14" s="3"/>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="3"/>
+      <c r="AN14" s="2"/>
+    </row>
+    <row r="15" spans="18:55">
+      <c r="R15" s="3"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="AI15" s="3"/>
+      <c r="AJ15" s="3"/>
+      <c r="AK15" s="3"/>
+      <c r="AL15" s="2"/>
+      <c r="AM15" s="3"/>
+      <c r="AN15" s="2"/>
+    </row>
+    <row r="16" spans="18:55">
+      <c r="R16" s="3"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="AI16" s="3"/>
+      <c r="AJ16" s="3"/>
+      <c r="AK16" s="3"/>
+      <c r="AL16" s="2"/>
+      <c r="AM16" s="3"/>
+      <c r="AN16" s="2"/>
+    </row>
+    <row r="17" spans="18:40">
+      <c r="R17" s="3"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="AI17" s="3"/>
+      <c r="AJ17" s="3"/>
+      <c r="AK17" s="3"/>
+      <c r="AL17" s="2"/>
+      <c r="AM17" s="3"/>
+      <c r="AN17" s="2"/>
+    </row>
+    <row r="18" spans="18:40">
+      <c r="R18" s="3"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="AI18" s="3"/>
+      <c r="AJ18" s="3"/>
+      <c r="AK18" s="3"/>
+      <c r="AL18" s="2"/>
+      <c r="AM18" s="3"/>
+      <c r="AN18" s="2"/>
+    </row>
+    <row r="19" spans="18:40">
+      <c r="R19" s="3"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="AI19" s="3"/>
+      <c r="AJ19" s="3"/>
+      <c r="AK19" s="3"/>
+      <c r="AL19" s="2"/>
+      <c r="AM19" s="3"/>
+      <c r="AN19" s="2"/>
+    </row>
+    <row r="20" spans="18:40">
+      <c r="R20" s="3"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="AI20" s="3"/>
+      <c r="AJ20" s="3"/>
+      <c r="AK20" s="3"/>
+      <c r="AL20" s="2"/>
+      <c r="AM20" s="3"/>
+      <c r="AN20" s="2"/>
+    </row>
+    <row r="21" spans="18:40">
+      <c r="R21" s="3"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="AI21" s="3"/>
+      <c r="AJ21" s="3"/>
+      <c r="AK21" s="3"/>
+      <c r="AL21" s="2"/>
+      <c r="AM21" s="3"/>
+      <c r="AN21" s="2"/>
+    </row>
+    <row r="22" spans="18:40">
+      <c r="R22" s="3"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Y22" s="3"/>
+      <c r="AI22" s="3"/>
+      <c r="AJ22" s="3"/>
+      <c r="AK22" s="3"/>
+      <c r="AL22" s="2"/>
+      <c r="AM22" s="3"/>
+      <c r="AN22" s="2"/>
+    </row>
+    <row r="23" spans="18:40">
+      <c r="R23" s="3"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="AI23" s="3"/>
+      <c r="AJ23" s="3"/>
+      <c r="AK23" s="3"/>
+      <c r="AL23" s="2"/>
+      <c r="AM23" s="3"/>
+      <c r="AN23" s="2"/>
+    </row>
+    <row r="24" spans="18:40">
+      <c r="R24" s="3"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3"/>
+      <c r="AK24" s="3"/>
+      <c r="AL24" s="2"/>
+      <c r="AM24" s="3"/>
+      <c r="AN24" s="2"/>
+    </row>
+    <row r="25" spans="18:40">
+      <c r="R25" s="3"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="AF25" s="2"/>
+      <c r="AG25" s="2"/>
+      <c r="AH25" s="3"/>
+      <c r="AI25" s="3"/>
+      <c r="AJ25" s="3"/>
+      <c r="AK25" s="3"/>
+      <c r="AL25" s="2"/>
+      <c r="AM25" s="3"/>
+      <c r="AN25" s="2"/>
+    </row>
+    <row r="26" spans="18:40">
+      <c r="R26" s="3"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="AF26" s="2"/>
+      <c r="AG26" s="2"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
+      <c r="AJ26" s="3"/>
+      <c r="AK26" s="3"/>
+      <c r="AL26" s="2"/>
+      <c r="AM26" s="3"/>
+      <c r="AN26" s="2"/>
+    </row>
+    <row r="27" spans="18:40">
+      <c r="R27" s="3"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="AF27" s="2"/>
+      <c r="AG27" s="2"/>
+      <c r="AH27" s="3"/>
+      <c r="AI27" s="3"/>
+      <c r="AJ27" s="3"/>
+      <c r="AK27" s="3"/>
+      <c r="AL27" s="2"/>
+      <c r="AM27" s="3"/>
+      <c r="AN27" s="2"/>
+    </row>
+    <row r="28" spans="18:40">
+      <c r="R28" s="3"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="AF28" s="2"/>
+      <c r="AG28" s="2"/>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="3"/>
+      <c r="AJ28" s="3"/>
+      <c r="AK28" s="3"/>
+      <c r="AL28" s="2"/>
+      <c r="AM28" s="3"/>
+      <c r="AN28" s="2"/>
+    </row>
+    <row r="29" spans="18:40">
+      <c r="R29" s="3"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="AF29" s="2"/>
+      <c r="AG29" s="2"/>
+      <c r="AH29" s="3"/>
+      <c r="AI29" s="3"/>
+      <c r="AJ29" s="3"/>
+      <c r="AK29" s="3"/>
+      <c r="AL29" s="2"/>
+      <c r="AM29" s="3"/>
+      <c r="AN29" s="2"/>
+    </row>
+    <row r="30" spans="18:40">
+      <c r="R30" s="3"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="3"/>
+      <c r="AF30" s="2"/>
+      <c r="AG30" s="2"/>
+      <c r="AH30" s="3"/>
+      <c r="AI30" s="3"/>
+      <c r="AJ30" s="3"/>
+      <c r="AK30" s="3"/>
+      <c r="AL30" s="2"/>
+      <c r="AM30" s="3"/>
+      <c r="AN30" s="2"/>
+    </row>
+    <row r="31" spans="18:40">
+      <c r="R31" s="3"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="AF31" s="2"/>
+      <c r="AG31" s="2"/>
+      <c r="AH31" s="3"/>
+      <c r="AI31" s="3"/>
+      <c r="AJ31" s="3"/>
+      <c r="AK31" s="3"/>
+      <c r="AL31" s="2"/>
+      <c r="AM31" s="3"/>
+      <c r="AN31" s="2"/>
+    </row>
+    <row r="32" spans="18:40">
+      <c r="R32" s="3"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="AF32" s="2"/>
+      <c r="AG32" s="2"/>
+      <c r="AH32" s="3"/>
+      <c r="AI32" s="3"/>
+      <c r="AJ32" s="3"/>
+      <c r="AK32" s="3"/>
+      <c r="AL32" s="2"/>
+      <c r="AM32" s="3"/>
+      <c r="AN32" s="2"/>
+    </row>
+    <row r="33" spans="1:40">
+      <c r="R33" s="3"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AA33" s="2"/>
+      <c r="AB33" s="2"/>
+      <c r="AC33" s="2"/>
+      <c r="AD33" s="3"/>
+      <c r="AE33" s="3"/>
+      <c r="AF33" s="2"/>
+      <c r="AG33" s="2"/>
+      <c r="AH33" s="3"/>
+      <c r="AI33" s="3"/>
+      <c r="AJ33" s="3"/>
+      <c r="AK33" s="3"/>
+      <c r="AL33" s="2"/>
+      <c r="AM33" s="3"/>
+      <c r="AN33" s="2"/>
+    </row>
+    <row r="34" spans="1:40">
+      <c r="R34" s="3"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="3"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3"/>
+      <c r="AA34" s="2"/>
+      <c r="AB34" s="2"/>
+      <c r="AC34" s="2"/>
+      <c r="AD34" s="3"/>
+      <c r="AE34" s="3"/>
+      <c r="AF34" s="2"/>
+      <c r="AG34" s="2"/>
+      <c r="AH34" s="3"/>
+      <c r="AI34" s="3"/>
+      <c r="AJ34" s="3"/>
+      <c r="AK34" s="3"/>
+      <c r="AL34" s="2"/>
+      <c r="AM34" s="3"/>
+      <c r="AN34" s="2"/>
+    </row>
+    <row r="35" spans="1:40">
+      <c r="R35" s="3"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="3"/>
+      <c r="U35" s="3"/>
+      <c r="V35" s="3"/>
+      <c r="W35" s="3"/>
+      <c r="X35" s="3"/>
+      <c r="Y35" s="3"/>
+      <c r="Z35" s="3"/>
+      <c r="AA35" s="2"/>
+      <c r="AB35" s="2"/>
+      <c r="AC35" s="2"/>
+      <c r="AD35" s="3"/>
+      <c r="AE35" s="3"/>
+      <c r="AF35" s="2"/>
+      <c r="AG35" s="2"/>
+      <c r="AH35" s="3"/>
+      <c r="AI35" s="3"/>
+      <c r="AJ35" s="3"/>
+      <c r="AK35" s="3"/>
+      <c r="AL35" s="2"/>
+      <c r="AM35" s="3"/>
+      <c r="AN35" s="2"/>
+    </row>
+    <row r="36" spans="1:40">
+      <c r="R36" s="3"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="3"/>
+      <c r="U36" s="3"/>
+      <c r="V36" s="3"/>
+      <c r="W36" s="3"/>
+      <c r="X36" s="3"/>
+      <c r="Y36" s="3"/>
+      <c r="Z36" s="3"/>
+      <c r="AA36" s="2"/>
+      <c r="AB36" s="2"/>
+      <c r="AC36" s="2"/>
+      <c r="AD36" s="3"/>
+      <c r="AE36" s="3"/>
+      <c r="AF36" s="2"/>
+      <c r="AG36" s="2"/>
+      <c r="AH36" s="3"/>
+      <c r="AI36" s="3"/>
+      <c r="AJ36" s="3"/>
+      <c r="AK36" s="3"/>
+      <c r="AL36" s="2"/>
+      <c r="AM36" s="3"/>
+      <c r="AN36" s="2"/>
+    </row>
+    <row r="37" spans="1:40">
+      <c r="A37" s="3"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="3"/>
+      <c r="U37" s="3"/>
+      <c r="V37" s="3"/>
+      <c r="W37" s="3"/>
+      <c r="X37" s="3"/>
+      <c r="Y37" s="3"/>
+      <c r="Z37" s="3"/>
+      <c r="AA37" s="2"/>
+      <c r="AB37" s="2"/>
+      <c r="AC37" s="2"/>
+      <c r="AD37" s="3"/>
+      <c r="AE37" s="3"/>
+      <c r="AF37" s="2"/>
+      <c r="AG37" s="2"/>
+      <c r="AH37" s="3"/>
+      <c r="AI37" s="3"/>
+      <c r="AJ37" s="3"/>
+      <c r="AK37" s="3"/>
+      <c r="AL37" s="2"/>
+      <c r="AM37" s="3"/>
+      <c r="AN37" s="2"/>
+    </row>
+    <row r="38" spans="1:40">
+      <c r="A38" s="3"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="3"/>
+      <c r="U38" s="3"/>
+      <c r="V38" s="3"/>
+      <c r="W38" s="3"/>
+      <c r="X38" s="3"/>
+      <c r="Y38" s="3"/>
+      <c r="Z38" s="3"/>
+      <c r="AA38" s="2"/>
+      <c r="AB38" s="2"/>
+      <c r="AC38" s="2"/>
+      <c r="AD38" s="3"/>
+      <c r="AE38" s="3"/>
+      <c r="AF38" s="2"/>
+      <c r="AG38" s="2"/>
+      <c r="AH38" s="3"/>
+      <c r="AI38" s="3"/>
+      <c r="AJ38" s="3"/>
+      <c r="AK38" s="3"/>
+      <c r="AL38" s="2"/>
+      <c r="AM38" s="3"/>
+      <c r="AN38" s="2"/>
+    </row>
+    <row r="39" spans="1:40">
+      <c r="A39" s="3"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="3"/>
+      <c r="U39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
+      <c r="Y39" s="3"/>
+      <c r="Z39" s="3"/>
+      <c r="AA39" s="2"/>
+      <c r="AB39" s="2"/>
+      <c r="AC39" s="2"/>
+      <c r="AD39" s="3"/>
+      <c r="AE39" s="3"/>
+      <c r="AF39" s="2"/>
+      <c r="AG39" s="2"/>
+      <c r="AH39" s="3"/>
+      <c r="AI39" s="3"/>
+      <c r="AJ39" s="3"/>
+      <c r="AK39" s="3"/>
+      <c r="AL39" s="2"/>
+      <c r="AM39" s="3"/>
+      <c r="AN39" s="2"/>
+    </row>
+    <row r="40" spans="1:40">
+      <c r="A40" s="3"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="3"/>
+      <c r="U40" s="3"/>
+      <c r="V40" s="3"/>
+      <c r="W40" s="3"/>
+      <c r="X40" s="3"/>
+      <c r="Y40" s="3"/>
+      <c r="Z40" s="3"/>
+      <c r="AA40" s="2"/>
+      <c r="AB40" s="2"/>
+      <c r="AC40" s="2"/>
+      <c r="AD40" s="3"/>
+      <c r="AE40" s="3"/>
+      <c r="AF40" s="2"/>
+      <c r="AG40" s="2"/>
+      <c r="AH40" s="3"/>
+      <c r="AI40" s="3"/>
+      <c r="AJ40" s="3"/>
+      <c r="AK40" s="3"/>
+      <c r="AL40" s="2"/>
+      <c r="AM40" s="3"/>
+      <c r="AN40" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>